<commit_message>
Working source code for location file generation.i
</commit_message>
<xml_diff>
--- a/documentations/AIR_OED_ValueMap_CEDEtoFile.xlsx
+++ b/documentations/AIR_OED_ValueMap_CEDEtoFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Subhashis Barik\Xceedance\Validating CAT Models\Model Evaluation Tool\Oasis_Modex\AIR-OED\Noida\Final Files\CEDE_To_File\ToShivam_CEDEtoFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3266AD8-CC9C-48D1-8205-41191D7D7124}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867C11EA-A5CC-4877-B7AA-E0E4B7886B5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="886" firstSheet="2" activeTab="6" xr2:uid="{9E8DA3F4-2086-4F29-9CE1-6E20884A5917}"/>
   </bookViews>
@@ -502,7 +502,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="746">
   <si>
     <t>AIR</t>
   </si>
@@ -2653,6 +2653,93 @@
   </si>
   <si>
     <t>xxxx</t>
+  </si>
+  <si>
+    <t>OED PerilText</t>
+  </si>
+  <si>
+    <t>AIR Peril Text</t>
+  </si>
+  <si>
+    <t>WTC</t>
+  </si>
+  <si>
+    <t>XSL;XTD;XHL</t>
+  </si>
+  <si>
+    <t>QEQ</t>
+  </si>
+  <si>
+    <t>QFF</t>
+  </si>
+  <si>
+    <t>WSS</t>
+  </si>
+  <si>
+    <t>MNT;MTR</t>
+  </si>
+  <si>
+    <t>ZST;ZSN;ZIC;ZFZ</t>
+  </si>
+  <si>
+    <t>QSL</t>
+  </si>
+  <si>
+    <t>BBF</t>
+  </si>
+  <si>
+    <t>ORF;OSF</t>
+  </si>
+  <si>
+    <t>QTS</t>
+  </si>
+  <si>
+    <t>BFR</t>
+  </si>
+  <si>
+    <t>QLS</t>
+  </si>
+  <si>
+    <t>QLF</t>
+  </si>
+  <si>
+    <t>PWX</t>
+  </si>
+  <si>
+    <t>PES</t>
+  </si>
+  <si>
+    <t>PFF</t>
+  </si>
+  <si>
+    <t>PSH</t>
+  </si>
+  <si>
+    <t>PTR</t>
+  </si>
+  <si>
+    <t>PWW</t>
+  </si>
+  <si>
+    <t>PSL</t>
+  </si>
+  <si>
+    <t>PWB</t>
+  </si>
+  <si>
+    <t>PFL</t>
+  </si>
+  <si>
+    <t>PTS</t>
+  </si>
+  <si>
+    <t>PNC</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t>PPH</t>
   </si>
 </sst>
 </file>
@@ -2841,7 +2928,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -3537,12 +3624,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3968,7 +4068,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3981,21 +4080,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4014,6 +4104,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4029,21 +4134,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4109,6 +4199,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4737,37 +4845,37 @@
       <c r="N3" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="Q3" s="184" t="s">
+      <c r="Q3" s="175" t="s">
         <v>133</v>
       </c>
-      <c r="R3" s="185"/>
-      <c r="S3" s="185"/>
-      <c r="T3" s="185"/>
-      <c r="U3" s="185"/>
-      <c r="V3" s="185"/>
-      <c r="W3" s="186"/>
-      <c r="X3" s="184" t="s">
+      <c r="R3" s="176"/>
+      <c r="S3" s="176"/>
+      <c r="T3" s="176"/>
+      <c r="U3" s="176"/>
+      <c r="V3" s="176"/>
+      <c r="W3" s="177"/>
+      <c r="X3" s="175" t="s">
         <v>134</v>
       </c>
-      <c r="Y3" s="185"/>
-      <c r="Z3" s="185"/>
-      <c r="AA3" s="186"/>
+      <c r="Y3" s="176"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="177"/>
     </row>
     <row r="4" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="181" t="s">
+      <c r="B4" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="183"/>
-      <c r="G4" s="181" t="s">
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="184"/>
+      <c r="G4" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="182"/>
-      <c r="I4" s="182"/>
-      <c r="J4" s="182"/>
-      <c r="K4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183"/>
+      <c r="K4" s="184"/>
       <c r="N4" t="s">
         <v>119</v>
       </c>
@@ -5342,14 +5450,14 @@
       <c r="B18" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="N18" s="187" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" s="188"/>
-      <c r="P18" s="187" t="s">
+      <c r="N18" s="178" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="179"/>
+      <c r="P18" s="178" t="s">
         <v>1</v>
       </c>
-      <c r="Q18" s="188"/>
+      <c r="Q18" s="179"/>
     </row>
     <row r="19" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="34" t="s">
@@ -5363,14 +5471,14 @@
       <c r="F19" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="N19" s="179" t="s">
+      <c r="N19" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="180"/>
-      <c r="P19" s="179" t="s">
+      <c r="O19" s="181"/>
+      <c r="P19" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="Q19" s="180"/>
+      <c r="Q19" s="181"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
@@ -5632,14 +5740,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="Q3:W3"/>
     <mergeCell ref="X3:AA3"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="N19:O19"/>
     <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="Q3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -5835,90 +5943,90 @@
       <c r="AI4" s="42"/>
     </row>
     <row r="5" spans="1:35" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="189" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="190"/>
-      <c r="C5" s="190"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="190"/>
-      <c r="F5" s="190"/>
-      <c r="G5" s="190"/>
-      <c r="H5" s="190"/>
-      <c r="I5" s="190"/>
-      <c r="J5" s="190"/>
-      <c r="K5" s="190"/>
-      <c r="L5" s="190"/>
-      <c r="M5" s="190"/>
-      <c r="N5" s="191"/>
-      <c r="O5" s="192" t="s">
+      <c r="A5" s="185" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="186"/>
+      <c r="C5" s="186"/>
+      <c r="D5" s="186"/>
+      <c r="E5" s="186"/>
+      <c r="F5" s="186"/>
+      <c r="G5" s="186"/>
+      <c r="H5" s="186"/>
+      <c r="I5" s="186"/>
+      <c r="J5" s="186"/>
+      <c r="K5" s="186"/>
+      <c r="L5" s="186"/>
+      <c r="M5" s="186"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="193"/>
-      <c r="Q5" s="193"/>
-      <c r="R5" s="193"/>
-      <c r="S5" s="193"/>
-      <c r="T5" s="193"/>
-      <c r="U5" s="193"/>
-      <c r="V5" s="193"/>
-      <c r="W5" s="193"/>
-      <c r="X5" s="193"/>
-      <c r="Y5" s="193"/>
-      <c r="Z5" s="193"/>
-      <c r="AA5" s="193"/>
-      <c r="AB5" s="193"/>
-      <c r="AC5" s="193"/>
-      <c r="AD5" s="193"/>
-      <c r="AE5" s="193"/>
-      <c r="AF5" s="193"/>
-      <c r="AG5" s="193"/>
-      <c r="AH5" s="193"/>
-      <c r="AI5" s="194"/>
+      <c r="P5" s="189"/>
+      <c r="Q5" s="189"/>
+      <c r="R5" s="189"/>
+      <c r="S5" s="189"/>
+      <c r="T5" s="189"/>
+      <c r="U5" s="189"/>
+      <c r="V5" s="189"/>
+      <c r="W5" s="189"/>
+      <c r="X5" s="189"/>
+      <c r="Y5" s="189"/>
+      <c r="Z5" s="189"/>
+      <c r="AA5" s="189"/>
+      <c r="AB5" s="189"/>
+      <c r="AC5" s="189"/>
+      <c r="AD5" s="189"/>
+      <c r="AE5" s="189"/>
+      <c r="AF5" s="189"/>
+      <c r="AG5" s="189"/>
+      <c r="AH5" s="189"/>
+      <c r="AI5" s="190"/>
     </row>
     <row r="6" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="195" t="s">
+      <c r="A6" s="191" t="s">
         <v>217</v>
       </c>
-      <c r="B6" s="196"/>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
-      <c r="E6" s="196"/>
-      <c r="F6" s="196"/>
-      <c r="G6" s="196"/>
-      <c r="H6" s="196"/>
-      <c r="I6" s="197"/>
-      <c r="J6" s="198" t="s">
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="193"/>
+      <c r="J6" s="194" t="s">
         <v>216</v>
       </c>
-      <c r="K6" s="196"/>
-      <c r="L6" s="196"/>
-      <c r="M6" s="196"/>
-      <c r="N6" s="199"/>
-      <c r="O6" s="200" t="s">
+      <c r="K6" s="192"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="192"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="196" t="s">
         <v>673</v>
       </c>
-      <c r="P6" s="201"/>
-      <c r="Q6" s="201"/>
-      <c r="R6" s="201"/>
-      <c r="S6" s="201"/>
-      <c r="T6" s="201"/>
-      <c r="U6" s="201"/>
-      <c r="V6" s="201"/>
-      <c r="W6" s="201"/>
-      <c r="X6" s="202"/>
-      <c r="Y6" s="203" t="s">
+      <c r="P6" s="197"/>
+      <c r="Q6" s="197"/>
+      <c r="R6" s="197"/>
+      <c r="S6" s="197"/>
+      <c r="T6" s="197"/>
+      <c r="U6" s="197"/>
+      <c r="V6" s="197"/>
+      <c r="W6" s="197"/>
+      <c r="X6" s="198"/>
+      <c r="Y6" s="199" t="s">
         <v>672</v>
       </c>
-      <c r="Z6" s="201"/>
-      <c r="AA6" s="201"/>
-      <c r="AB6" s="201"/>
-      <c r="AC6" s="201"/>
-      <c r="AD6" s="201"/>
-      <c r="AE6" s="201"/>
-      <c r="AF6" s="201"/>
-      <c r="AG6" s="201"/>
-      <c r="AH6" s="201"/>
-      <c r="AI6" s="204"/>
+      <c r="Z6" s="197"/>
+      <c r="AA6" s="197"/>
+      <c r="AB6" s="197"/>
+      <c r="AC6" s="197"/>
+      <c r="AD6" s="197"/>
+      <c r="AE6" s="197"/>
+      <c r="AF6" s="197"/>
+      <c r="AG6" s="197"/>
+      <c r="AH6" s="197"/>
+      <c r="AI6" s="200"/>
     </row>
     <row r="7" spans="1:35" s="130" customFormat="1" ht="144" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="141" t="s">
@@ -14758,24 +14866,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="208" t="s">
+      <c r="B1" s="204" t="s">
         <v>658</v>
       </c>
-      <c r="C1" s="209"/>
-      <c r="D1" s="210"/>
-      <c r="E1" s="205" t="s">
+      <c r="C1" s="205"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="201" t="s">
         <v>623</v>
       </c>
-      <c r="F1" s="206"/>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="206"/>
-      <c r="L1" s="206"/>
-      <c r="M1" s="206"/>
-      <c r="N1" s="206"/>
-      <c r="O1" s="207"/>
+      <c r="F1" s="202"/>
+      <c r="G1" s="202"/>
+      <c r="H1" s="202"/>
+      <c r="I1" s="202"/>
+      <c r="J1" s="202"/>
+      <c r="K1" s="202"/>
+      <c r="L1" s="202"/>
+      <c r="M1" s="202"/>
+      <c r="N1" s="202"/>
+      <c r="O1" s="203"/>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="147" t="s">
@@ -15351,289 +15459,422 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76528CA-6AB3-41BE-957D-8BDD4BC7B32A}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="30"/>
-    <col min="2" max="2" width="20.28515625" style="165" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="165" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="165" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="163"/>
-    <col min="6" max="16384" width="9.140625" style="20"/>
+    <col min="2" max="2" width="20.28515625" style="164" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="164" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="164" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="99.85546875" style="207" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="175" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="171" t="s">
         <v>690</v>
       </c>
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="171" t="s">
         <v>715</v>
       </c>
-      <c r="D2" s="176" t="s">
+      <c r="D2" s="172" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="167">
+      <c r="E2" s="171" t="s">
+        <v>717</v>
+      </c>
+      <c r="F2" s="208" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="166">
         <f>B9+B10+B14+B20+B18+B16</f>
         <v>139916</v>
       </c>
-      <c r="C3" s="178" t="s">
+      <c r="C3" s="174" t="s">
         <v>711</v>
       </c>
-      <c r="D3" s="168">
+      <c r="D3" s="174">
         <f>D9+D10+D14+D20+D18+D16</f>
         <v>262175</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="169">
+      <c r="E3" s="212" t="str">
+        <f>CONCATENATE(E9,";",E10,";",E14,";",E20,";",E18,";",E16)</f>
+        <v>QEQ;QFF;QSL;QLS;QTS;BBF</v>
+      </c>
+      <c r="F3" s="152" t="str">
+        <f>C3</f>
+        <v>PEA</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="167">
         <f>B22+B15+B7+B11</f>
         <v>4369</v>
       </c>
-      <c r="C4" s="166" t="s">
+      <c r="C4" s="165" t="s">
         <v>712</v>
       </c>
-      <c r="D4" s="170">
+      <c r="D4" s="165">
         <f>D22+D15+D7+D11</f>
         <v>2112</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="169">
+      <c r="E4" s="209" t="str">
+        <f>CONCATENATE(E22,";",E15,";",E7,";",E11)</f>
+        <v>ORF;OSF;WSS;WTC;WSS</v>
+      </c>
+      <c r="F4" s="154" t="str">
+        <f>C4</f>
+        <v>PPH+PSH+PWH</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="167">
         <f>B19+B8+B12+B13</f>
         <v>65634</v>
       </c>
-      <c r="C5" s="166" t="s">
+      <c r="C5" s="165" t="s">
         <v>713</v>
       </c>
-      <c r="D5" s="170">
+      <c r="D5" s="165">
         <f>D19+D8+D12+D13</f>
         <v>6027264</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="169">
+      <c r="E5" s="209" t="str">
+        <f>CONCATENATE(E19,";",E8,";",E12,";",E13)</f>
+        <v>BFR;XSL;XTD;XHL;MNT;MTR;ZST;ZSN;ZIC;ZFZ</v>
+      </c>
+      <c r="F5" s="154" t="str">
+        <f>C5</f>
+        <v>PNC+PWX+PTR</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="167">
         <f>B3+B4+B5+B17</f>
         <v>211967</v>
       </c>
-      <c r="C6" s="164" t="s">
+      <c r="C6" s="163" t="s">
         <v>714</v>
       </c>
-      <c r="D6" s="170">
+      <c r="D6" s="165">
         <f>D3+D4+D5+D17</f>
         <v>6293087</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="169">
+      <c r="E6" s="209" t="str">
+        <f>CONCATENATE(E3,";",E4,";",E5,";",E17)</f>
+        <v>QEQ;QFF;QSL;QLS;QTS;BBF;ORF;OSF;WSS;WTC;WSS;BFR;XSL;XTD;XHL;MNT;MTR;ZST;ZSN;ZIC;ZFZ;ORF;OSF</v>
+      </c>
+      <c r="F6" s="154" t="str">
+        <f>C6</f>
+        <v>PNC+PEA+PPH+PFL+PSH+PWA+PTR</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="167">
         <v>1</v>
       </c>
-      <c r="C7" s="164" t="s">
+      <c r="C7" s="163" t="s">
         <v>691</v>
       </c>
-      <c r="D7" s="170">
+      <c r="D7" s="165">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="169">
+      <c r="E7" s="209" t="s">
+        <v>719</v>
+      </c>
+      <c r="F7" s="154" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="167">
         <v>2</v>
       </c>
-      <c r="C8" s="164" t="s">
+      <c r="C8" s="163" t="s">
         <v>692</v>
       </c>
-      <c r="D8" s="170">
+      <c r="D8" s="165">
         <v>14336</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="169">
+      <c r="E8" s="209" t="s">
+        <v>720</v>
+      </c>
+      <c r="F8" s="154" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="167">
         <v>4</v>
       </c>
-      <c r="C9" s="164" t="s">
+      <c r="C9" s="163" t="s">
         <v>693</v>
       </c>
-      <c r="D9" s="170">
+      <c r="D9" s="165">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="169">
+      <c r="E9" s="209" t="s">
+        <v>721</v>
+      </c>
+      <c r="F9" s="154" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="167">
         <v>8</v>
       </c>
-      <c r="C10" s="164" t="s">
+      <c r="C10" s="163" t="s">
         <v>694</v>
       </c>
-      <c r="D10" s="170">
+      <c r="D10" s="165">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="169">
+      <c r="E10" s="209" t="s">
+        <v>722</v>
+      </c>
+      <c r="F10" s="154" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="167">
         <v>16</v>
       </c>
-      <c r="C11" s="164" t="s">
+      <c r="C11" s="163" t="s">
         <v>695</v>
       </c>
-      <c r="D11" s="170">
+      <c r="D11" s="165">
         <v>256</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="169">
+      <c r="E11" s="209" t="s">
+        <v>723</v>
+      </c>
+      <c r="F11" s="154" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="167">
         <v>32</v>
       </c>
-      <c r="C12" s="164" t="s">
+      <c r="C12" s="163" t="s">
         <v>696</v>
       </c>
-      <c r="D12" s="170">
+      <c r="D12" s="165">
         <v>1572864</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="169">
+      <c r="E12" s="209" t="s">
+        <v>724</v>
+      </c>
+      <c r="F12" s="154" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="167">
         <v>64</v>
       </c>
-      <c r="C13" s="164" t="s">
+      <c r="C13" s="163" t="s">
         <v>697</v>
       </c>
-      <c r="D13" s="170">
+      <c r="D13" s="165">
         <v>4308992</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="169">
+      <c r="E13" s="209" t="s">
+        <v>725</v>
+      </c>
+      <c r="F13" s="154" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="167">
         <v>128</v>
       </c>
-      <c r="C14" s="164" t="s">
+      <c r="C14" s="163" t="s">
         <v>698</v>
       </c>
-      <c r="D14" s="170">
+      <c r="D14" s="165">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="169">
+      <c r="E14" s="209" t="s">
+        <v>726</v>
+      </c>
+      <c r="F14" s="154" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="167">
         <v>256</v>
       </c>
-      <c r="C15" s="164" t="s">
+      <c r="C15" s="163" t="s">
         <v>699</v>
       </c>
-      <c r="D15" s="170">
+      <c r="D15" s="165">
         <v>256</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="169">
+      <c r="E15" s="209" t="s">
+        <v>723</v>
+      </c>
+      <c r="F15" s="154" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="167">
         <v>512</v>
       </c>
-      <c r="C16" s="164" t="s">
+      <c r="C16" s="163" t="s">
         <v>700</v>
       </c>
-      <c r="D16" s="170">
+      <c r="D16" s="165">
         <v>262144</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="169">
+      <c r="E16" s="209" t="s">
+        <v>727</v>
+      </c>
+      <c r="F16" s="154" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="167">
         <v>2048</v>
       </c>
-      <c r="C17" s="164" t="s">
+      <c r="C17" s="163" t="s">
         <v>701</v>
       </c>
-      <c r="D17" s="170">
+      <c r="D17" s="165">
         <v>1536</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="169">
+      <c r="E17" s="209" t="s">
+        <v>728</v>
+      </c>
+      <c r="F17" s="154" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="167">
         <v>8192</v>
       </c>
-      <c r="C18" s="164" t="s">
+      <c r="C18" s="163" t="s">
         <v>247</v>
       </c>
-      <c r="D18" s="170">
+      <c r="D18" s="165">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="169">
+      <c r="E18" s="209" t="s">
+        <v>729</v>
+      </c>
+      <c r="F18" s="154" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="167">
         <v>65536</v>
       </c>
-      <c r="C19" s="164" t="s">
+      <c r="C19" s="163" t="s">
         <v>702</v>
       </c>
-      <c r="D19" s="170">
+      <c r="D19" s="165">
         <v>131072</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="169">
+      <c r="E19" s="209" t="s">
+        <v>730</v>
+      </c>
+      <c r="F19" s="154" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="167">
         <v>131072</v>
       </c>
-      <c r="C20" s="164" t="s">
+      <c r="C20" s="163" t="s">
         <v>703</v>
       </c>
-      <c r="D20" s="170">
+      <c r="D20" s="165">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="169">
+      <c r="E20" s="209" t="s">
+        <v>731</v>
+      </c>
+      <c r="F20" s="154" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="167">
         <v>4194304</v>
       </c>
-      <c r="C21" s="164" t="s">
+      <c r="C21" s="163" t="s">
         <v>704</v>
       </c>
-      <c r="D21" s="170">
+      <c r="D21" s="165">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="171">
+      <c r="E21" s="209" t="s">
+        <v>732</v>
+      </c>
+      <c r="F21" s="154"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="168">
         <v>4096</v>
       </c>
-      <c r="C22" s="177" t="s">
+      <c r="C22" s="173" t="s">
         <v>705</v>
       </c>
-      <c r="D22" s="172">
+      <c r="D22" s="210">
         <v>1536</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="174" t="s">
+      <c r="E22" s="211" t="s">
+        <v>728</v>
+      </c>
+      <c r="F22" s="156" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="170" t="s">
         <v>710</v>
       </c>
-      <c r="C23" s="174" t="s">
+      <c r="C23" s="170" t="s">
         <v>716</v>
       </c>
-      <c r="D23" s="174" t="s">
+      <c r="D23" s="170" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
     </row>
   </sheetData>
@@ -15730,7 +15971,7 @@
       </c>
     </row>
     <row r="11" spans="2:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="173" t="s">
+      <c r="B11" s="169" t="s">
         <v>707</v>
       </c>
       <c r="C11" s="30" t="s">

</xml_diff>